<commit_message>
Test Cases for Search Funtionality done
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\SQA Projects\Chaldal.com Assignment\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1B0694-9B08-4DA7-B395-D602B6962D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{68EA14D2-858B-4358-9C5A-F33BFF21A1F9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Summary" sheetId="2" r:id="rId1"/>
     <sheet name="Test Cases" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -55,13 +49,151 @@
   </si>
   <si>
     <t>Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                Test Cases for Search Functionality</t>
+  </si>
+  <si>
+    <t>TC_SF_001</t>
+  </si>
+  <si>
+    <t>Check functionality with blank value</t>
+  </si>
+  <si>
+    <t>TC_SF_002</t>
+  </si>
+  <si>
+    <t>Check search functionality with only space</t>
+  </si>
+  <si>
+    <t>TC_SF_003</t>
+  </si>
+  <si>
+    <t>Check search functionality with special characters</t>
+  </si>
+  <si>
+    <t>TC_SF_004</t>
+  </si>
+  <si>
+    <t>Check search functionality with invalid product name</t>
+  </si>
+  <si>
+    <t>TC_SF_005</t>
+  </si>
+  <si>
+    <t>Check search functionality with only number</t>
+  </si>
+  <si>
+    <t>TC_SF_006</t>
+  </si>
+  <si>
+    <t>Check search functionality with valid product name</t>
+  </si>
+  <si>
+    <t>TC_SF_007</t>
+  </si>
+  <si>
+    <t>Search results displayed should be relevant to search keyword</t>
+  </si>
+  <si>
+    <t>% sign in search keyword should not redirect to 404 ERROR</t>
+  </si>
+  <si>
+    <t>Application should not crash if user inserted % in search field</t>
+  </si>
+  <si>
+    <t>When user start typing word in text box it should suggest words that matches typed keyword</t>
+  </si>
+  <si>
+    <t>There should be pre-defined search criteria for auto complete e.g. after typing first 3 letter it should suggest matching keyword</t>
+  </si>
+  <si>
+    <t>When user clicks on any link from result and navigates back, then result should be maintained</t>
+  </si>
+  <si>
+    <t>After clicking Search field - search history should be displayed (latest search keyword)</t>
+  </si>
+  <si>
+    <t>All search keyword/filters should get cleared on clicking Reset button</t>
+  </si>
+  <si>
+    <t>Search results should be cleared on clicking clear search button</t>
+  </si>
+  <si>
+    <t>History displayed in search field should be relevant to logged in user only</t>
+  </si>
+  <si>
+    <t>Pagination should be tested for searches returning high number of records</t>
+  </si>
+  <si>
+    <t>Total number of search records/results should be displayed on page</t>
+  </si>
+  <si>
+    <t>Search keyword should get highlighted with color in the search results</t>
+  </si>
+  <si>
+    <t>search keyword should suggest similar kind of product/items</t>
+  </si>
+  <si>
+    <t>User should be able to search when he enters the keyword and hits ‘Enter’ button on keyboard</t>
+  </si>
+  <si>
+    <t>TC_SF_009</t>
+  </si>
+  <si>
+    <t>TC_SF_010</t>
+  </si>
+  <si>
+    <t>TC_SF_011</t>
+  </si>
+  <si>
+    <t>TC_SF_012</t>
+  </si>
+  <si>
+    <t>TC_SF_013</t>
+  </si>
+  <si>
+    <t>TC_SF_014</t>
+  </si>
+  <si>
+    <t>TC_SF_015</t>
+  </si>
+  <si>
+    <t>TC_SF_016</t>
+  </si>
+  <si>
+    <t>TC_SF_017</t>
+  </si>
+  <si>
+    <t>TC_SF_018</t>
+  </si>
+  <si>
+    <t>TC_SF_019</t>
+  </si>
+  <si>
+    <t>TC_SF_020</t>
+  </si>
+  <si>
+    <t>TC_SF_021</t>
+  </si>
+  <si>
+    <t>TC_SF_022</t>
+  </si>
+  <si>
+    <t>TC_SF_023</t>
+  </si>
+  <si>
+    <t>TC_SF_024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                Test Cases for Order System Functionality</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,8 +209,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,6 +227,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -119,10 +264,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -184,7 +351,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -236,7 +403,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -430,14 +597,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{053505A9-1D90-4297-A339-0F990F01DE88}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -449,18 +616,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55F0EF4-42BE-41F2-BFF3-44DB2FDFA412}">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.54296875" customWidth="1"/>
-    <col min="2" max="2" width="43.54296875" customWidth="1"/>
+    <col min="2" max="2" width="43.54296875" style="8" customWidth="1"/>
     <col min="3" max="3" width="26.1796875" customWidth="1"/>
     <col min="4" max="4" width="17.6328125" customWidth="1"/>
     <col min="5" max="5" width="26.81640625" customWidth="1"/>
@@ -491,7 +658,212 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="3" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="3" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A30:G30"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test case design for order system
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -177,12 +177,6 @@
     <t>TC_SF_022</t>
   </si>
   <si>
-    <t>TC_SF_023</t>
-  </si>
-  <si>
-    <t>TC_SF_024</t>
-  </si>
-  <si>
     <t xml:space="preserve">                                                Test Cases for Login System Functionality</t>
   </si>
   <si>
@@ -271,6 +265,97 @@
   </si>
   <si>
     <t>TC_LF_014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                Test Cases for Order System Functionality</t>
+  </si>
+  <si>
+    <t>TC_Order_001</t>
+  </si>
+  <si>
+    <t>Verify that the user can add to cart one or more products.</t>
+  </si>
+  <si>
+    <t>Verify that users can add products to the wishlist.</t>
+  </si>
+  <si>
+    <t>Verify that the user can buy products added to the cart after signing in to the application.</t>
+  </si>
+  <si>
+    <t>Verify that the user can successfully buy more than one product that was added to his/her cart.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the user cannot add more than the available inventory of the product.
+</t>
+  </si>
+  <si>
+    <t>Verify that the limit to the number of products a user can by is working correctly by displaying an error message and preventing the user from buying more than the limit.</t>
+  </si>
+  <si>
+    <t>Verify that the Cash on Delivery option of payment is working fine.</t>
+  </si>
+  <si>
+    <t>Verify that the different pre-paid methods of payments are working fine.</t>
+  </si>
+  <si>
+    <t>Check that it is possible to add items to the cart and continue shopping</t>
+  </si>
+  <si>
+    <t>Check that If the user adds the same item to the cart while continuing to shop, the item count in the shopping cart should get incremented</t>
+  </si>
+  <si>
+    <t>All items and their totals should be displayed in the cart</t>
+  </si>
+  <si>
+    <t>Check that Remove items from the cart working perfectly.</t>
+  </si>
+  <si>
+    <t>Check that Apply coupon function working fine.</t>
+  </si>
+  <si>
+    <t>Don’t check out, close the site, and come back later. The site should retain the items in the cart</t>
+  </si>
+  <si>
+    <t>TC_Order_002</t>
+  </si>
+  <si>
+    <t>TC_Order_003</t>
+  </si>
+  <si>
+    <t>TC_Order_004</t>
+  </si>
+  <si>
+    <t>TC_Order_005</t>
+  </si>
+  <si>
+    <t>TC_Order_006</t>
+  </si>
+  <si>
+    <t>TC_Order_007</t>
+  </si>
+  <si>
+    <t>TC_Order_008</t>
+  </si>
+  <si>
+    <t>TC_Order_009</t>
+  </si>
+  <si>
+    <t>TC_Order_010</t>
+  </si>
+  <si>
+    <t>TC_Order_011</t>
+  </si>
+  <si>
+    <t>TC_Order_012</t>
+  </si>
+  <si>
+    <t>TC_Order_013</t>
+  </si>
+  <si>
+    <t>TC_Order_014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                Test Cases for Payment System</t>
   </si>
 </sst>
 </file>
@@ -321,7 +406,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -342,17 +427,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -386,13 +460,13 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -701,7 +775,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -721,20 +795,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.54296875" customWidth="1"/>
-    <col min="2" max="2" width="43.54296875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="48.81640625" style="7" customWidth="1"/>
     <col min="3" max="3" width="26.1796875" customWidth="1"/>
     <col min="4" max="4" width="17.6328125" customWidth="1"/>
-    <col min="5" max="5" width="26.81640625" customWidth="1"/>
+    <col min="5" max="5" width="22.08984375" customWidth="1"/>
     <col min="6" max="6" width="17.36328125" customWidth="1"/>
     <col min="7" max="7" width="17.54296875" customWidth="1"/>
   </cols>
@@ -759,7 +833,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -942,18 +1016,14 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="A26" s="2"/>
     </row>
     <row r="27" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="A27" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -964,121 +1034,257 @@
     </row>
     <row r="32" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B32" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B35" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="36" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B36" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="37" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B37" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B38" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="39" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B39" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="40" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B40" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="41" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B41" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B42" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="43" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B43" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="44" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>77</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B44" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="45" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B45" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="46" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B44" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+    </row>
+    <row r="50" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="30.5" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="B50" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>101</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>102</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>103</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>104</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>105</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>106</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>107</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A66" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A48:G48"/>
+    <mergeCell ref="A66:G66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Test case design for Payment system
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -356,6 +356,51 @@
   </si>
   <si>
     <t xml:space="preserve">                                                Test Cases for Payment System</t>
+  </si>
+  <si>
+    <t>TC_Payment_001</t>
+  </si>
+  <si>
+    <t>Check that different payment options are available or not.</t>
+  </si>
+  <si>
+    <t>If allowing check out as Guest, simply finish the purchase and provide an option to register at the end</t>
+  </si>
+  <si>
+    <t>If the user is signed up for a long time, make sure the session is timed out or not.</t>
+  </si>
+  <si>
+    <t>TC_LF_015</t>
+  </si>
+  <si>
+    <t>Check that after order Emails/Text confirmation with the order number generated or not.</t>
+  </si>
+  <si>
+    <t>Check that payment with bKash and other mobile banking is possible or not.</t>
+  </si>
+  <si>
+    <t>Check that wrong address accept or not.</t>
+  </si>
+  <si>
+    <t>Check that cash on delivery is available or not.</t>
+  </si>
+  <si>
+    <t>TC_Payment_002</t>
+  </si>
+  <si>
+    <t>TC_Payment_003</t>
+  </si>
+  <si>
+    <t>TC_Payment_004</t>
+  </si>
+  <si>
+    <t>TC_Payment_005</t>
+  </si>
+  <si>
+    <t>TC_Payment_006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                Test Cases for Order Cancelation</t>
   </si>
 </sst>
 </file>
@@ -459,7 +504,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -469,6 +513,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -775,7 +820,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -795,11 +840,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A68" sqref="A68"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -837,15 +882,15 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
@@ -1018,273 +1063,337 @@
     <row r="26" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="9" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-    </row>
-    <row r="32" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+    </row>
+    <row r="30" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>67</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>54</v>
+        <v>69</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>68</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>55</v>
+        <v>70</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>69</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>56</v>
+        <v>71</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>57</v>
+        <v>72</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>58</v>
+        <v>73</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>72</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>59</v>
+        <v>74</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>73</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>60</v>
+        <v>75</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>74</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>61</v>
+        <v>76</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>75</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>77</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>78</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-    </row>
-    <row r="50" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+    </row>
+    <row r="48" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>95</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>104</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>106</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>107</v>
-      </c>
-      <c r="B63" s="8" t="s">
         <v>94</v>
       </c>
     </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+    </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A66" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B66" s="9"/>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
+      <c r="A66" t="s">
+        <v>109</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>118</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>119</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>120</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>121</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>122</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A74" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A48:G48"/>
-    <mergeCell ref="A66:G66"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="A64:G64"/>
+    <mergeCell ref="A74:G74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Test case execution for Searching functionality
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="158">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Test Case Title</t>
   </si>
   <si>
-    <t>Step Description</t>
-  </si>
-  <si>
     <t>Test Data</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>When user start typing word in text box it should suggest words that matches typed keyword</t>
   </si>
   <si>
-    <t>There should be pre-defined search criteria for auto complete e.g. after typing first 3 letter it should suggest matching keyword</t>
-  </si>
-  <si>
     <t>When user clicks on any link from result and navigates back, then result should be maintained</t>
   </si>
   <si>
@@ -114,12 +108,6 @@
     <t>All search keyword/filters should get cleared on clicking Reset button</t>
   </si>
   <si>
-    <t>Search results should be cleared on clicking clear search button</t>
-  </si>
-  <si>
-    <t>History displayed in search field should be relevant to logged in user only</t>
-  </si>
-  <si>
     <t>Pagination should be tested for searches returning high number of records</t>
   </si>
   <si>
@@ -165,21 +153,6 @@
     <t>TC_SF_018</t>
   </si>
   <si>
-    <t>TC_SF_019</t>
-  </si>
-  <si>
-    <t>TC_SF_020</t>
-  </si>
-  <si>
-    <t>TC_SF_021</t>
-  </si>
-  <si>
-    <t>TC_SF_022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                Test Cases for Login System Functionality</t>
-  </si>
-  <si>
     <t>TC_LF_001</t>
   </si>
   <si>
@@ -265,9 +238,6 @@
   </si>
   <si>
     <t>TC_LF_014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                Test Cases for Order System Functionality</t>
   </si>
   <si>
     <t>TC_Order_001</t>
@@ -401,13 +371,145 @@
   </si>
   <si>
     <t xml:space="preserve">                                                Test Cases for Order Cancelation</t>
+  </si>
+  <si>
+    <t>TC_OC_001</t>
+  </si>
+  <si>
+    <t>Check that order change is possible or not</t>
+  </si>
+  <si>
+    <t>Check that cancel order is possible or not.</t>
+  </si>
+  <si>
+    <t>Check that online order tracking is possible or not.</t>
+  </si>
+  <si>
+    <t>TC_OC_002</t>
+  </si>
+  <si>
+    <t>TC_OC_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                Test Cases for Login/Signup Functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                Test Cases for Shopping Cart &amp; Order System Functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                Test Cases for Product Details Page</t>
+  </si>
+  <si>
+    <t>TC_PDP_001</t>
+  </si>
+  <si>
+    <t>Check that product name display or not.</t>
+  </si>
+  <si>
+    <t>Check that product price display or not.</t>
+  </si>
+  <si>
+    <t>Check that product details display or not.</t>
+  </si>
+  <si>
+    <t>Check that check-out option available on details page.</t>
+  </si>
+  <si>
+    <t>Check that total number of stock product information is available.</t>
+  </si>
+  <si>
+    <t>Check that zoom view is working or not.</t>
+  </si>
+  <si>
+    <t>Check that user can rate, review the product</t>
+  </si>
+  <si>
+    <t>TC_PDP_002</t>
+  </si>
+  <si>
+    <t>TC_PDP_003</t>
+  </si>
+  <si>
+    <t>TC_PDP_004</t>
+  </si>
+  <si>
+    <t>TC_PDP_005</t>
+  </si>
+  <si>
+    <t>TC_PDP_006</t>
+  </si>
+  <si>
+    <t>TC_PDP_007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                Test Cases for miscellaneous functionalities</t>
+  </si>
+  <si>
+    <t>TC_M_001</t>
+  </si>
+  <si>
+    <t>Check the Language change functionality</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/158_AhpZIIMNbdZ6RyQzMchY0owJ2mTyw/view</t>
+  </si>
+  <si>
+    <t>TC_M_002</t>
+  </si>
+  <si>
+    <t>Check chat box by sending only space</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1RA06mWMmr0d-SyoUKhtaZV49i0pqMFPy/view</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1xO7GrgfrTcEs-lTEHayDidXaBBy7mtYg/view</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/16FPvkjzTuSLUR6tagBMgBrjxjBhS-VlN/view</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1lD3hwcJe9zA7g1973ELWo-snND2VbxuJ/view</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1aUemR_6RvjUYm1WTsqu6Q8wXEtmLWAzE/view</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1azT_2T6OpedpLiW2sGH6-dWOI39KM5oH/view</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/18Eh5FCAr6zlcWadT2RJZaqRHdo32ltWC/view</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1p2i_WmXMSA8TMwGGJCzTReedYlNmPQUZ/view</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1WILg8LQE3MEJEMo17vwK5Y9Bg9YM1x2s/view</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/12pFso_mor7ep1aGQK4lNsYICxTmeVzeu/view</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/14Ag9URQLtnbqvm56aJPpDZbHGRPRf1vM/view</t>
+  </si>
+  <si>
+    <t>TC_SF_008</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -430,8 +532,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1" tint="0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -447,6 +571,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -475,10 +611,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -514,8 +651,24 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -820,7 +973,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -840,22 +993,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A76" sqref="A76"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.54296875" customWidth="1"/>
-    <col min="2" max="2" width="48.81640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="44.90625" style="7" customWidth="1"/>
     <col min="3" max="3" width="26.1796875" customWidth="1"/>
     <col min="4" max="4" width="17.6328125" customWidth="1"/>
     <col min="5" max="5" width="22.08984375" customWidth="1"/>
     <col min="6" max="6" width="17.36328125" customWidth="1"/>
-    <col min="7" max="7" width="17.54296875" customWidth="1"/>
+    <col min="7" max="7" width="22.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="46" customHeight="1" x14ac:dyDescent="0.35">
@@ -875,15 +1028,15 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>52</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -892,510 +1045,720 @@
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="F5" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="G5" s="16"/>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="F6" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="F7" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="F8" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="F9" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="F10" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="56" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="F11" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="F12" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="56" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="B17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="B18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="B19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="61" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="B20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="B21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="B22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+    </row>
+    <row r="27" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="B27" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+    </row>
+    <row r="28" spans="1:7" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+    </row>
+    <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+    </row>
+    <row r="30" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+    </row>
+    <row r="31" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>47</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-    </row>
-    <row r="30" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>66</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>75</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>76</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>77</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>64</v>
+        <v>103</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>78</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>113</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
+      <c r="A43" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+    </row>
+    <row r="45" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>95</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>103</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F57" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G57" s="13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>97</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>99</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>108</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>109</v>
+      </c>
+      <c r="B65" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B58" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+    </row>
+    <row r="66" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>110</v>
+      </c>
+      <c r="B66" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B59" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>111</v>
+      </c>
+      <c r="B67" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B60" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>112</v>
+      </c>
+      <c r="B68" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B61" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A64" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>109</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A71" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>114</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
         <v>118</v>
       </c>
-      <c r="B67" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
+      <c r="B74" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
         <v>119</v>
       </c>
-      <c r="B68" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>120</v>
-      </c>
-      <c r="B69" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>121</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
+      <c r="B75" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A78" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B71" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A74" s="12" t="s">
+      <c r="B78" s="12"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="12"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
         <v>123</v>
       </c>
-      <c r="B74" s="12"/>
-      <c r="C74" s="12"/>
-      <c r="D74" s="12"/>
-      <c r="E74" s="12"/>
-      <c r="F74" s="12"/>
-      <c r="G74" s="12"/>
+      <c r="B80" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>131</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>132</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>133</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>134</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>135</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>136</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B90" s="12"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="12"/>
+      <c r="E90" s="12"/>
+      <c r="F90" s="12"/>
+      <c r="G90" s="12"/>
+    </row>
+    <row r="92" spans="1:7" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>138</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F92" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G92" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>143</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F93" s="15" t="s">
+        <v>146</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A78:G78"/>
+    <mergeCell ref="A90:G90"/>
     <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A64:G64"/>
-    <mergeCell ref="A74:G74"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A43:G43"/>
+    <mergeCell ref="A61:G61"/>
+    <mergeCell ref="A71:G71"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G92" r:id="rId1"/>
+    <hyperlink ref="G57" r:id="rId2"/>
+    <hyperlink ref="G21" r:id="rId3"/>
+    <hyperlink ref="G6" r:id="rId4"/>
+    <hyperlink ref="G7" r:id="rId5"/>
+    <hyperlink ref="G8" r:id="rId6"/>
+    <hyperlink ref="G9" r:id="rId7"/>
+    <hyperlink ref="G14" r:id="rId8"/>
+    <hyperlink ref="G16" r:id="rId9"/>
+    <hyperlink ref="G17" r:id="rId10"/>
+    <hyperlink ref="G18" r:id="rId11"/>
+    <hyperlink ref="G19" r:id="rId12"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test case execution for Login/Signup functionality
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="158">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -615,7 +615,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -624,9 +624,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -635,12 +632,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -650,7 +641,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -660,11 +650,37 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -973,7 +989,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -996,14 +1012,14 @@
   <dimension ref="A1:G93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.54296875" customWidth="1"/>
-    <col min="2" max="2" width="44.90625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="44.90625" style="4" customWidth="1"/>
     <col min="3" max="3" width="26.1796875" customWidth="1"/>
     <col min="4" max="4" width="17.6328125" customWidth="1"/>
     <col min="5" max="5" width="22.08984375" customWidth="1"/>
@@ -1015,7 +1031,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1046,25 +1062,31 @@
       <c r="G3" s="12"/>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="15" t="s">
         <v>146</v>
       </c>
       <c r="G5" s="16"/>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="17" t="s">
         <v>141</v>
       </c>
       <c r="G6" s="16" t="s">
@@ -1072,207 +1094,262 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="2" customFormat="1" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="17" t="s">
         <v>141</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:7" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="21" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="21" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="17" t="s">
-        <v>146</v>
-      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="G10" s="22"/>
     </row>
     <row r="11" spans="1:7" ht="56" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="17" t="s">
-        <v>146</v>
-      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="G11" s="22"/>
     </row>
     <row r="12" spans="1:7" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="17" t="s">
-        <v>146</v>
-      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="G12" s="22"/>
     </row>
     <row r="13" spans="1:7" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="17" t="s">
-        <v>146</v>
-      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="G13" s="22"/>
     </row>
     <row r="14" spans="1:7" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="21" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="56" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="17" t="s">
-        <v>146</v>
-      </c>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="G15" s="22"/>
     </row>
     <row r="16" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="21" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="21" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="21" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="21" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="61" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="17" t="s">
-        <v>146</v>
-      </c>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="G20" s="22"/>
     </row>
     <row r="21" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="21" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="17" t="s">
-        <v>146</v>
-      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="G22" s="22"/>
     </row>
     <row r="23" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
@@ -1288,124 +1365,169 @@
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
     </row>
-    <row r="27" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F27" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="6" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F28" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F29" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F30" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F31" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F32" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="59" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F33" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="60.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="7" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F34" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F35" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F36" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F37" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="53" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F38" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F39" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>69</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="8" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F40" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>103</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="5" t="s">
         <v>102</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -1423,7 +1545,7 @@
       <c r="A45" t="s">
         <v>70</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1431,7 +1553,7 @@
       <c r="A46" t="s">
         <v>85</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="4" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1439,7 +1561,7 @@
       <c r="A47" t="s">
         <v>86</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="5" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1447,7 +1569,7 @@
       <c r="A48" t="s">
         <v>87</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="5" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1455,7 +1577,7 @@
       <c r="A49" t="s">
         <v>88</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="5" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1463,7 +1585,7 @@
       <c r="A50" t="s">
         <v>89</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="5" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1471,7 +1593,7 @@
       <c r="A51" t="s">
         <v>90</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="5" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1479,7 +1601,7 @@
       <c r="A52" t="s">
         <v>91</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="5" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1487,7 +1609,7 @@
       <c r="A53" t="s">
         <v>92</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="5" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1495,7 +1617,7 @@
       <c r="A54" t="s">
         <v>93</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="5" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1503,7 +1625,7 @@
       <c r="A55" t="s">
         <v>94</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1511,21 +1633,21 @@
       <c r="A56" t="s">
         <v>95</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" ht="68" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>96</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F57" s="14" t="s">
+      <c r="F57" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="G57" s="13" t="s">
+      <c r="G57" s="9" t="s">
         <v>145</v>
       </c>
     </row>
@@ -1533,7 +1655,7 @@
       <c r="A58" t="s">
         <v>97</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" s="5" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1552,15 +1674,15 @@
       <c r="A63" t="s">
         <v>99</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B63" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>108</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B64" s="5" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1568,7 +1690,7 @@
       <c r="A65" t="s">
         <v>109</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B65" s="5" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1576,7 +1698,7 @@
       <c r="A66" t="s">
         <v>110</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B66" s="5" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1584,7 +1706,7 @@
       <c r="A67" t="s">
         <v>111</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B67" s="4" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1592,7 +1714,7 @@
       <c r="A68" t="s">
         <v>112</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B68" s="4" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1611,7 +1733,7 @@
       <c r="A73" t="s">
         <v>114</v>
       </c>
-      <c r="B73" s="7" t="s">
+      <c r="B73" s="4" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1619,7 +1741,7 @@
       <c r="A74" t="s">
         <v>118</v>
       </c>
-      <c r="B74" s="7" t="s">
+      <c r="B74" s="4" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1627,7 +1749,7 @@
       <c r="A75" t="s">
         <v>119</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="B75" s="4" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1646,7 +1768,7 @@
       <c r="A80" t="s">
         <v>123</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="B80" s="4" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1654,7 +1776,7 @@
       <c r="A81" t="s">
         <v>131</v>
       </c>
-      <c r="B81" s="7" t="s">
+      <c r="B81" s="4" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1662,7 +1784,7 @@
       <c r="A82" t="s">
         <v>132</v>
       </c>
-      <c r="B82" s="7" t="s">
+      <c r="B82" s="4" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1670,7 +1792,7 @@
       <c r="A83" t="s">
         <v>133</v>
       </c>
-      <c r="B83" s="7" t="s">
+      <c r="B83" s="4" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1678,7 +1800,7 @@
       <c r="A84" t="s">
         <v>134</v>
       </c>
-      <c r="B84" s="8" t="s">
+      <c r="B84" s="5" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1686,7 +1808,7 @@
       <c r="A85" t="s">
         <v>135</v>
       </c>
-      <c r="B85" s="7" t="s">
+      <c r="B85" s="4" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1694,7 +1816,7 @@
       <c r="A86" t="s">
         <v>136</v>
       </c>
-      <c r="B86" s="7" t="s">
+      <c r="B86" s="4" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1713,13 +1835,13 @@
       <c r="A92" t="s">
         <v>138</v>
       </c>
-      <c r="B92" s="7" t="s">
+      <c r="B92" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="F92" s="14" t="s">
+      <c r="F92" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="G92" s="13" t="s">
+      <c r="G92" s="9" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1727,10 +1849,10 @@
       <c r="A93" t="s">
         <v>143</v>
       </c>
-      <c r="B93" s="7" t="s">
+      <c r="B93" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="F93" s="15" t="s">
+      <c r="F93" s="11" t="s">
         <v>146</v>
       </c>
     </row>

</xml_diff>

<commit_message>
almost 90% Test case execution complete
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="163">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -265,12 +265,6 @@
     <t>Verify that the Cash on Delivery option of payment is working fine.</t>
   </si>
   <si>
-    <t>Verify that the different pre-paid methods of payments are working fine.</t>
-  </si>
-  <si>
-    <t>Check that it is possible to add items to the cart and continue shopping</t>
-  </si>
-  <si>
     <t>Check that If the user adds the same item to the cart while continuing to shop, the item count in the shopping cart should get incremented</t>
   </si>
   <si>
@@ -304,12 +298,6 @@
     <t>TC_Order_007</t>
   </si>
   <si>
-    <t>TC_Order_008</t>
-  </si>
-  <si>
-    <t>TC_Order_009</t>
-  </si>
-  <si>
     <t>TC_Order_010</t>
   </si>
   <si>
@@ -503,6 +491,33 @@
   </si>
   <si>
     <t>TC_SF_008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                Test Cases for User's Profile Section</t>
+  </si>
+  <si>
+    <t>TC_UP_001</t>
+  </si>
+  <si>
+    <t>Check update profile with invalid address</t>
+  </si>
+  <si>
+    <t>Check "Your Orders" tab display all orders history</t>
+  </si>
+  <si>
+    <t>Check "Payment History" tab display all payments history</t>
+  </si>
+  <si>
+    <t>Check change password functionality works properly</t>
+  </si>
+  <si>
+    <t>TC_M_003</t>
+  </si>
+  <si>
+    <t>Check all the links under "Help" menu is navigate to the proper page.</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1dC_INBkRlDX8ZtgxaxF4k7GPgdW3EJdE/view</t>
   </si>
 </sst>
 </file>
@@ -615,7 +630,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -629,28 +644,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -681,6 +674,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -989,7 +992,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1009,16 +1012,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G93"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" style="2" customWidth="1"/>
     <col min="2" max="2" width="44.90625" style="4" customWidth="1"/>
     <col min="3" max="3" width="26.1796875" customWidth="1"/>
     <col min="4" max="4" width="17.6328125" customWidth="1"/>
@@ -1031,7 +1034,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1047,828 +1050,1165 @@
         <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="15" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="G5" s="16"/>
-    </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="G6" s="16" t="s">
+    </row>
+    <row r="9" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:7" ht="56" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:7" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:7" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="1:7" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G14" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="G7" s="16" t="s">
+    <row r="15" spans="1:7" ht="56" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G16" s="13" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="G8" s="21" t="s">
+    <row r="17" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G17" s="13" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="G9" s="21" t="s">
+    <row r="18" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G18" s="13" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="G10" s="22"/>
-    </row>
-    <row r="11" spans="1:7" ht="56" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="G11" s="22"/>
-    </row>
-    <row r="12" spans="1:7" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="G12" s="22"/>
-    </row>
-    <row r="13" spans="1:7" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="G13" s="22"/>
-    </row>
-    <row r="14" spans="1:7" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="G14" s="21" t="s">
+    <row r="19" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G19" s="13" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="56" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="G15" s="22"/>
-    </row>
-    <row r="16" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="G17" s="21" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="G18" s="21" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>156</v>
-      </c>
-    </row>
     <row r="20" spans="1:7" ht="61" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="G20" s="22"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G20" s="14"/>
     </row>
     <row r="21" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="G21" s="21" t="s">
-        <v>147</v>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="G22" s="22"/>
-    </row>
-    <row r="23" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
-    </row>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
+      <c r="A25" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
     </row>
     <row r="27" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="A27" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F27" s="15" t="s">
-        <v>146</v>
-      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="A28" s="5" t="s">
         <v>57</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F28" s="15" t="s">
-        <v>146</v>
-      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="A29" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F29" s="15" t="s">
-        <v>146</v>
-      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="A30" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F30" s="15" t="s">
-        <v>146</v>
-      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G30" s="14"/>
     </row>
     <row r="31" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="A31" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F31" s="15" t="s">
-        <v>146</v>
-      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="A32" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F32" s="15" t="s">
-        <v>146</v>
-      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G32" s="14"/>
     </row>
     <row r="33" spans="1:7" ht="59" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+      <c r="A33" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F33" s="15" t="s">
-        <v>146</v>
-      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G33" s="14"/>
     </row>
     <row r="34" spans="1:7" ht="60.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="A34" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="F34" s="15" t="s">
-        <v>146</v>
-      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G34" s="14"/>
     </row>
     <row r="35" spans="1:7" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="A35" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F35" s="15" t="s">
-        <v>146</v>
-      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G35" s="14"/>
     </row>
     <row r="36" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="A36" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="F36" s="15" t="s">
-        <v>146</v>
-      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G36" s="14"/>
     </row>
     <row r="37" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="A37" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F37" s="15" t="s">
-        <v>146</v>
-      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G37" s="14"/>
     </row>
     <row r="38" spans="1:7" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+      <c r="A38" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F38" s="15" t="s">
-        <v>146</v>
-      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G38" s="14"/>
     </row>
     <row r="39" spans="1:7" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="A39" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="F39" s="15" t="s">
-        <v>146</v>
-      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G39" s="14"/>
     </row>
     <row r="40" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="A40" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="F40" s="15" t="s">
-        <v>146</v>
-      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G40" s="14"/>
     </row>
     <row r="41" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+      <c r="A41" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G41" s="14"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+    </row>
+    <row r="45" spans="1:7" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G45" s="14"/>
+    </row>
+    <row r="46" spans="1:7" ht="62" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G46" s="14"/>
+    </row>
+    <row r="47" spans="1:7" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G47" s="14"/>
+    </row>
+    <row r="48" spans="1:7" ht="69.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G48" s="14"/>
+    </row>
+    <row r="49" spans="1:7" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G49" s="14"/>
+    </row>
+    <row r="50" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A50" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G50" s="14"/>
+    </row>
+    <row r="51" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G51" s="14"/>
+    </row>
+    <row r="52" spans="1:7" ht="62" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G52" s="14"/>
+    </row>
+    <row r="53" spans="1:7" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G53" s="14"/>
+    </row>
+    <row r="54" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G54" s="14"/>
+    </row>
+    <row r="55" spans="1:7" ht="68" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G55" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G56" s="14"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B59" s="16"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="16"/>
+    </row>
+    <row r="61" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G61" s="14"/>
+    </row>
+    <row r="62" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G62" s="14"/>
+    </row>
+    <row r="63" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G63" s="14"/>
+    </row>
+    <row r="64" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G64" s="14"/>
+    </row>
+    <row r="65" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G65" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="F41" s="15" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="12" t="s">
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G66" s="14"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B69" s="16"/>
+      <c r="C69" s="16"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="16"/>
+      <c r="G69" s="16"/>
+    </row>
+    <row r="71" spans="1:7" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G71" s="14"/>
+    </row>
+    <row r="72" spans="1:7" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G72" s="14"/>
+    </row>
+    <row r="73" spans="1:7" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="14"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A74" s="5"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="14"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A76" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B76" s="16"/>
+      <c r="C76" s="16"/>
+      <c r="D76" s="16"/>
+      <c r="E76" s="16"/>
+      <c r="F76" s="16"/>
+      <c r="G76" s="16"/>
+    </row>
+    <row r="78" spans="1:7" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G78" s="14"/>
+    </row>
+    <row r="79" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B79" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-    </row>
-    <row r="45" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>70</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>85</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>86</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>87</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>88</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>89</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>90</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>91</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>92</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>93</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>94</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>95</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="68" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>96</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F57" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="G57" s="9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>97</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A61" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="B61" s="12"/>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>99</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>108</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>109</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>110</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>111</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>112</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A71" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
-      <c r="G71" s="12"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>114</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>118</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>119</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A78" s="12" t="s">
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G79" s="14"/>
+    </row>
+    <row r="80" spans="1:7" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B80" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="B78" s="12"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="12"/>
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
-      <c r="G78" s="12"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G80" s="14"/>
+    </row>
+    <row r="81" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B81" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="C81" s="14"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G81" s="14"/>
+    </row>
+    <row r="82" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B82" s="11" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
+      <c r="C82" s="14"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G82" s="14"/>
+    </row>
+    <row r="83" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B83" s="6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G83" s="14"/>
+    </row>
+    <row r="84" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B84" s="6" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
+      <c r="C84" s="14"/>
+      <c r="D84" s="14"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G84" s="14"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B87" s="16"/>
+      <c r="C87" s="16"/>
+      <c r="D87" s="16"/>
+      <c r="E87" s="16"/>
+      <c r="F87" s="16"/>
+      <c r="G87" s="16"/>
+    </row>
+    <row r="89" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G89" s="14"/>
+    </row>
+    <row r="90" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G90" s="14"/>
+    </row>
+    <row r="91" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B91" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C91" s="14"/>
+      <c r="D91" s="14"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G91" s="14"/>
+    </row>
+    <row r="92" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C92" s="14"/>
+      <c r="D92" s="14"/>
+      <c r="E92" s="14"/>
+      <c r="F92" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G92" s="14"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A95" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B83" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
+      <c r="B95" s="16"/>
+      <c r="C95" s="16"/>
+      <c r="D95" s="16"/>
+      <c r="E95" s="16"/>
+      <c r="F95" s="16"/>
+      <c r="G95" s="16"/>
+    </row>
+    <row r="97" spans="1:7" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B84" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+      <c r="B97" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B85" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
-        <v>136</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A90" s="12" t="s">
+      <c r="C97" s="14"/>
+      <c r="D97" s="14"/>
+      <c r="E97" s="14"/>
+      <c r="F97" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B90" s="12"/>
-      <c r="C90" s="12"/>
-      <c r="D90" s="12"/>
-      <c r="E90" s="12"/>
-      <c r="F90" s="12"/>
-      <c r="G90" s="12"/>
-    </row>
-    <row r="92" spans="1:7" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
+      <c r="G97" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="B92" s="4" t="s">
+    </row>
+    <row r="98" spans="1:7" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="F92" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="G92" s="9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
-        <v>143</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F93" s="11" t="s">
-        <v>146</v>
-      </c>
+      <c r="B98" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C98" s="14"/>
+      <c r="D98" s="14"/>
+      <c r="E98" s="14"/>
+      <c r="F98" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G98" s="14"/>
+    </row>
+    <row r="99" spans="1:7" ht="68" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B99" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C99" s="14"/>
+      <c r="D99" s="14"/>
+      <c r="E99" s="14"/>
+      <c r="F99" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G99" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A78:G78"/>
-    <mergeCell ref="A90:G90"/>
+  <mergeCells count="8">
+    <mergeCell ref="A76:G76"/>
+    <mergeCell ref="A95:G95"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A25:G25"/>
     <mergeCell ref="A43:G43"/>
-    <mergeCell ref="A61:G61"/>
-    <mergeCell ref="A71:G71"/>
+    <mergeCell ref="A59:G59"/>
+    <mergeCell ref="A69:G69"/>
+    <mergeCell ref="A87:G87"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G92" r:id="rId1"/>
-    <hyperlink ref="G57" r:id="rId2"/>
+    <hyperlink ref="G97" r:id="rId1"/>
+    <hyperlink ref="G55" r:id="rId2"/>
     <hyperlink ref="G21" r:id="rId3"/>
     <hyperlink ref="G6" r:id="rId4"/>
     <hyperlink ref="G7" r:id="rId5"/>
@@ -1879,8 +2219,9 @@
     <hyperlink ref="G17" r:id="rId10"/>
     <hyperlink ref="G18" r:id="rId11"/>
     <hyperlink ref="G19" r:id="rId12"/>
+    <hyperlink ref="G65" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update Login Test cases
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="204">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -518,13 +518,142 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/1dC_INBkRlDX8ZtgxaxF4k7GPgdW3EJdE/view</t>
+  </si>
+  <si>
+    <t>Should display error message</t>
+  </si>
+  <si>
+    <t>Error message has displayed.</t>
+  </si>
+  <si>
+    <t>single space</t>
+  </si>
+  <si>
+    <t>should not display any product</t>
+  </si>
+  <si>
+    <t>Some product has displayed.</t>
+  </si>
+  <si>
+    <t>@', '#'</t>
+  </si>
+  <si>
+    <t>lul</t>
+  </si>
+  <si>
+    <t>milk</t>
+  </si>
+  <si>
+    <t>should display some product</t>
+  </si>
+  <si>
+    <t>right product has displayed</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>should not redirect</t>
+  </si>
+  <si>
+    <t>work perfectly</t>
+  </si>
+  <si>
+    <t>should not crash</t>
+  </si>
+  <si>
+    <t>properly handle</t>
+  </si>
+  <si>
+    <t>should give some suggestion</t>
+  </si>
+  <si>
+    <t>no suggestion has given</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
+  </si>
+  <si>
+    <t>search history should display</t>
+  </si>
+  <si>
+    <t>Not working</t>
+  </si>
+  <si>
+    <t>Reset button should available</t>
+  </si>
+  <si>
+    <t>There have no reset button</t>
+  </si>
+  <si>
+    <t>page pagination should available</t>
+  </si>
+  <si>
+    <t>There have no pagination available</t>
+  </si>
+  <si>
+    <t>search result's number should available</t>
+  </si>
+  <si>
+    <t>should be suggest similar kind of items</t>
+  </si>
+  <si>
+    <t>should be login</t>
+  </si>
+  <si>
+    <t>login has been successful</t>
+  </si>
+  <si>
+    <t>should not be login</t>
+  </si>
+  <si>
+    <t>Error message has displayed successfully.</t>
+  </si>
+  <si>
+    <t>Email : xyz@gmail.com
+Pass : 123456</t>
+  </si>
+  <si>
+    <t>Email : xyz#gmail.com
+Pass : 123456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email : xyz@gmail.com
+Pass : _ _ </t>
+  </si>
+  <si>
+    <t>Email : xyz#gmail.com
+Pass : 123____</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email: xyz@gmail.com
+Pass : </t>
+  </si>
+  <si>
+    <t>Email : @#$%^
+Pass : %^&amp;^%</t>
+  </si>
+  <si>
+    <t>should display proper error message</t>
+  </si>
+  <si>
+    <t>Error message has displayed properly</t>
+  </si>
+  <si>
+    <t>should display proper placeholders</t>
+  </si>
+  <si>
+    <t>displayed perfectly</t>
+  </si>
+  <si>
+    <t>working properly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -556,15 +685,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="24"/>
+      <sz val="14"/>
+      <color theme="1" tint="0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="0" tint="-0.14999847407452621"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="22"/>
-      <color theme="1" tint="0.14999847407452621"/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -630,7 +766,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -650,14 +786,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -675,15 +805,29 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -992,7 +1136,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1015,18 +1159,18 @@
   <dimension ref="A1:G99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C101" sqref="C101"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17.54296875" style="2" customWidth="1"/>
     <col min="2" max="2" width="44.90625" style="4" customWidth="1"/>
     <col min="3" max="3" width="26.1796875" customWidth="1"/>
-    <col min="4" max="4" width="17.6328125" customWidth="1"/>
-    <col min="5" max="5" width="22.08984375" customWidth="1"/>
-    <col min="6" max="6" width="17.36328125" customWidth="1"/>
+    <col min="4" max="4" width="17.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="24.7265625" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" style="19" customWidth="1"/>
     <col min="7" max="7" width="22.36328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1034,7 +1178,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1071,13 +1215,19 @@
       <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G5" s="8"/>
+      <c r="C5" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
@@ -1086,13 +1236,19 @@
       <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="9" t="s">
+      <c r="C6" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1103,30 +1259,42 @@
       <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="9" t="s">
+      <c r="C7" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F7" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="9" t="s">
+      <c r="C8" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="11" t="s">
         <v>146</v>
       </c>
     </row>
@@ -1137,13 +1305,19 @@
       <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="9" t="s">
+      <c r="C9" s="5">
+        <v>123</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F9" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="11" t="s">
         <v>147</v>
       </c>
     </row>
@@ -1154,73 +1328,95 @@
       <c r="B10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G10" s="14"/>
+      <c r="C10" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" ht="56" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G11" s="14"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:7" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G12" s="14"/>
+      <c r="C12" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:7" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G13" s="14"/>
+      <c r="C13" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="9" t="s">
+      <c r="C14" s="12"/>
+      <c r="D14" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="F14" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="11" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1228,31 +1424,41 @@
       <c r="A15" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G15" s="14"/>
+      <c r="C15" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="9" t="s">
+      <c r="C16" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="F16" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="11" t="s">
         <v>149</v>
       </c>
     </row>
@@ -1260,16 +1466,22 @@
       <c r="A17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="9" t="s">
+      <c r="C17" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="F17" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="11" t="s">
         <v>150</v>
       </c>
     </row>
@@ -1277,16 +1489,22 @@
       <c r="A18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="9" t="s">
+      <c r="C18" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="F18" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="11" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1294,16 +1512,22 @@
       <c r="A19" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="9" t="s">
+      <c r="C19" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="F19" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="11" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1311,31 +1535,39 @@
       <c r="A20" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G20" s="14"/>
+      <c r="C20" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="9" t="s">
+      <c r="C21" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F21" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="11" t="s">
         <v>143</v>
       </c>
     </row>
@@ -1343,19 +1575,21 @@
       <c r="A22" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G22" s="14"/>
-    </row>
-    <row r="23" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C22" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="25" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A25" s="16" t="s">
         <v>116</v>
       </c>
@@ -1373,13 +1607,19 @@
       <c r="B27" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G27" s="14"/>
+      <c r="C27" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G27" s="12"/>
     </row>
     <row r="28" spans="1:7" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
@@ -1388,210 +1628,284 @@
       <c r="B28" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G28" s="14"/>
+      <c r="C28" s="5">
+        <v>1682706635</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G28" s="12"/>
     </row>
     <row r="29" spans="1:7" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G29" s="14"/>
+      <c r="C29" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G29" s="12"/>
     </row>
     <row r="30" spans="1:7" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G30" s="14"/>
+      <c r="C30" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G30" s="12"/>
     </row>
     <row r="31" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G31" s="14"/>
+      <c r="C31" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G31" s="12"/>
     </row>
     <row r="32" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G32" s="14"/>
+      <c r="C32" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G32" s="12"/>
     </row>
     <row r="33" spans="1:7" ht="59" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G33" s="14"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G33" s="12"/>
     </row>
     <row r="34" spans="1:7" ht="60.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G34" s="14"/>
+      <c r="C34" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G34" s="12"/>
     </row>
     <row r="35" spans="1:7" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G35" s="14"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G35" s="12"/>
     </row>
     <row r="36" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G36" s="14"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G36" s="12"/>
     </row>
     <row r="37" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G37" s="14"/>
+      <c r="C37" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G37" s="12"/>
     </row>
     <row r="38" spans="1:7" ht="53" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G38" s="14"/>
+      <c r="C38" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G38" s="12"/>
     </row>
     <row r="39" spans="1:7" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G39" s="14"/>
+      <c r="C39" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G39" s="12"/>
     </row>
     <row r="40" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G40" s="14"/>
+      <c r="C40" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G40" s="12"/>
     </row>
     <row r="41" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G41" s="14"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C41" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D41" s="5"/>
+      <c r="E41" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G41" s="12"/>
+    </row>
+    <row r="43" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A43" s="16" t="s">
         <v>117</v>
       </c>
@@ -1606,16 +1920,16 @@
       <c r="A45" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G45" s="14"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G45" s="12"/>
     </row>
     <row r="46" spans="1:7" ht="62" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
@@ -1624,133 +1938,133 @@
       <c r="B46" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G46" s="14"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G46" s="12"/>
     </row>
     <row r="47" spans="1:7" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G47" s="14"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G47" s="12"/>
     </row>
     <row r="48" spans="1:7" ht="69.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G48" s="14"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G48" s="12"/>
     </row>
     <row r="49" spans="1:7" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G49" s="14"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G49" s="12"/>
     </row>
     <row r="50" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G50" s="14"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G50" s="12"/>
     </row>
     <row r="51" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G51" s="14"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G51" s="12"/>
     </row>
     <row r="52" spans="1:7" ht="62" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G52" s="14"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G52" s="12"/>
     </row>
     <row r="53" spans="1:7" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B53" s="11" t="s">
+      <c r="B53" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G53" s="14"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G53" s="12"/>
     </row>
     <row r="54" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="B54" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G54" s="14"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G54" s="12"/>
     </row>
     <row r="55" spans="1:7" ht="68" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
@@ -1759,13 +2073,13 @@
       <c r="B55" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="9" t="s">
+      <c r="C55" s="12"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G55" s="13" t="s">
+      <c r="G55" s="11" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1773,18 +2087,18 @@
       <c r="A56" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B56" s="11" t="s">
+      <c r="B56" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G56" s="14"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C56" s="12"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G56" s="12"/>
+    </row>
+    <row r="59" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A59" s="16" t="s">
         <v>94</v>
       </c>
@@ -1799,61 +2113,61 @@
       <c r="A61" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B61" s="11" t="s">
+      <c r="B61" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G61" s="14"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G61" s="12"/>
     </row>
     <row r="62" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B62" s="11" t="s">
+      <c r="B62" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G62" s="14"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G62" s="12"/>
     </row>
     <row r="63" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B63" s="11" t="s">
+      <c r="B63" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G63" s="14"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G63" s="12"/>
     </row>
     <row r="64" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B64" s="11" t="s">
+      <c r="B64" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G64" s="14"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G64" s="12"/>
     </row>
     <row r="65" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
@@ -1862,13 +2176,13 @@
       <c r="B65" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="9" t="s">
+      <c r="C65" s="12"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G65" s="18" t="s">
+      <c r="G65" s="15" t="s">
         <v>162</v>
       </c>
     </row>
@@ -1879,15 +2193,15 @@
       <c r="B66" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G66" s="14"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C66" s="12"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G66" s="12"/>
+    </row>
+    <row r="69" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A69" s="16" t="s">
         <v>109</v>
       </c>
@@ -1905,13 +2219,13 @@
       <c r="B71" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G71" s="14"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G71" s="12"/>
     </row>
     <row r="72" spans="1:7" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
@@ -1920,37 +2234,37 @@
       <c r="B72" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G72" s="14"/>
-    </row>
-    <row r="73" spans="1:7" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C72" s="12"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G72" s="12"/>
+    </row>
+    <row r="73" spans="1:7" ht="38" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="5" t="s">
         <v>115</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C73" s="14"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="14"/>
-      <c r="G73" s="14"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C73" s="12"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="20"/>
+      <c r="G73" s="12"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" s="5"/>
       <c r="B74" s="6"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
-      <c r="G74" s="14"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C74" s="12"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="20"/>
+      <c r="G74" s="12"/>
+    </row>
+    <row r="76" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A76" s="16" t="s">
         <v>118</v>
       </c>
@@ -1968,13 +2282,13 @@
       <c r="B78" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C78" s="14"/>
-      <c r="D78" s="14"/>
-      <c r="E78" s="14"/>
-      <c r="F78" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G78" s="14"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="G78" s="12"/>
     </row>
     <row r="79" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
@@ -1983,13 +2297,13 @@
       <c r="B79" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C79" s="14"/>
-      <c r="D79" s="14"/>
-      <c r="E79" s="14"/>
-      <c r="F79" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G79" s="14"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="G79" s="12"/>
     </row>
     <row r="80" spans="1:7" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
@@ -1998,13 +2312,13 @@
       <c r="B80" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C80" s="14"/>
-      <c r="D80" s="14"/>
-      <c r="E80" s="14"/>
-      <c r="F80" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G80" s="14"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="G80" s="12"/>
     </row>
     <row r="81" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
@@ -2013,28 +2327,28 @@
       <c r="B81" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C81" s="14"/>
-      <c r="D81" s="14"/>
-      <c r="E81" s="14"/>
-      <c r="F81" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G81" s="14"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="G81" s="12"/>
     </row>
     <row r="82" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B82" s="11" t="s">
+      <c r="B82" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="C82" s="14"/>
-      <c r="D82" s="14"/>
-      <c r="E82" s="14"/>
-      <c r="F82" s="9" t="s">
+      <c r="C82" s="12"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G82" s="14"/>
+      <c r="G82" s="12"/>
     </row>
     <row r="83" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
@@ -2043,13 +2357,13 @@
       <c r="B83" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C83" s="14"/>
-      <c r="D83" s="14"/>
-      <c r="E83" s="14"/>
-      <c r="F83" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G83" s="14"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="G83" s="12"/>
     </row>
     <row r="84" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
@@ -2058,15 +2372,15 @@
       <c r="B84" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C84" s="14"/>
-      <c r="D84" s="14"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="9" t="s">
+      <c r="C84" s="12"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G84" s="14"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G84" s="12"/>
+    </row>
+    <row r="87" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A87" s="16" t="s">
         <v>154</v>
       </c>
@@ -2084,13 +2398,13 @@
       <c r="B89" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="C89" s="14"/>
-      <c r="D89" s="14"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="9" t="s">
+      <c r="C89" s="12"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="12"/>
+      <c r="F89" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G89" s="14"/>
+      <c r="G89" s="12"/>
     </row>
     <row r="90" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
@@ -2099,28 +2413,28 @@
       <c r="B90" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="C90" s="14"/>
-      <c r="D90" s="14"/>
-      <c r="E90" s="14"/>
-      <c r="F90" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G90" s="14"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="12"/>
+      <c r="F90" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="G90" s="12"/>
     </row>
     <row r="91" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B91" s="11" t="s">
+      <c r="B91" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="C91" s="14"/>
-      <c r="D91" s="14"/>
-      <c r="E91" s="14"/>
-      <c r="F91" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G91" s="14"/>
+      <c r="C91" s="12"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="G91" s="12"/>
     </row>
     <row r="92" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
@@ -2129,15 +2443,15 @@
       <c r="B92" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C92" s="14"/>
-      <c r="D92" s="14"/>
-      <c r="E92" s="14"/>
-      <c r="F92" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G92" s="14"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C92" s="12"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="G92" s="12"/>
+    </row>
+    <row r="95" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A95" s="16" t="s">
         <v>133</v>
       </c>
@@ -2155,13 +2469,13 @@
       <c r="B97" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C97" s="14"/>
-      <c r="D97" s="14"/>
-      <c r="E97" s="14"/>
-      <c r="F97" s="9" t="s">
+      <c r="C97" s="12"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="12"/>
+      <c r="F97" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G97" s="13" t="s">
+      <c r="G97" s="11" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2172,28 +2486,28 @@
       <c r="B98" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C98" s="14"/>
-      <c r="D98" s="14"/>
-      <c r="E98" s="14"/>
-      <c r="F98" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G98" s="14"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="G98" s="12"/>
     </row>
     <row r="99" spans="1:7" ht="68" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B99" s="11" t="s">
+      <c r="B99" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="C99" s="14"/>
-      <c r="D99" s="14"/>
-      <c r="E99" s="14"/>
-      <c r="F99" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G99" s="14"/>
+      <c r="C99" s="12"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="12"/>
+      <c r="F99" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="G99" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>